<commit_message>
feat: Update staff data, app icon, and dashboard UI refactor
</commit_message>
<xml_diff>
--- a/통제단 웹앱용 직원 임무.xlsx
+++ b/통제단 웹앱용 직원 임무.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\코딩자료\통제단\control-center\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61743CE2-BB0E-4927-B375-7D25AE5573AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="직원별 임무" sheetId="2" r:id="rId1"/>
@@ -24,12 +25,15 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="240">
   <si>
     <t>통제단편성부</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -95,10 +99,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>김승일</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>김지영</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -135,10 +135,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>홍승민</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>소방사</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -155,10 +151,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>이동주</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>권순호</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -187,14 +179,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>박성철</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>김명선</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>이동찬</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -215,10 +199,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>진영재</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>이유진</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -255,10 +235,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>정상혁</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>현장대응단</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -283,10 +259,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>박민지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>양미주</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -308,10 +280,6 @@
   </si>
   <si>
     <t>김종철</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>김정석</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1017,11 +985,55 @@
     <t>구조구급주임</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>서창봉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>김도완</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>홍승진</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정장호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>김선화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>조은정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>박재권</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>김수연</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>임종래</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정재기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>김경국</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1093,7 +1105,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1123,6 +1135,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1403,11 +1418,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1425,7 +1440,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -1437,19 +1452,19 @@
         <v>2</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -1469,10 +1484,10 @@
         <v>5</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>8</v>
@@ -1493,16 +1508,16 @@
         <v>11</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="I3" s="3"/>
     </row>
@@ -1520,16 +1535,16 @@
         <v>13</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="I4" s="3"/>
     </row>
@@ -1543,18 +1558,20 @@
       <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>229</v>
+      </c>
       <c r="E5" s="3" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="I5" s="3"/>
     </row>
@@ -1569,19 +1586,19 @@
         <v>15</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>16</v>
+        <v>230</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="I6" s="3"/>
     </row>
@@ -1596,19 +1613,19 @@
         <v>12</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="I7" s="3"/>
     </row>
@@ -1623,19 +1640,19 @@
         <v>14</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="I8" s="3"/>
     </row>
@@ -1650,19 +1667,19 @@
         <v>15</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="I9" s="3"/>
     </row>
@@ -1671,25 +1688,25 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="I10" s="3"/>
     </row>
@@ -1698,25 +1715,25 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="I11" s="3"/>
     </row>
@@ -1725,25 +1742,25 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="I12" s="3"/>
     </row>
@@ -1752,25 +1769,25 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>26</v>
+        <v>231</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="I13" s="3"/>
     </row>
@@ -1779,25 +1796,25 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="I14" s="3"/>
     </row>
@@ -1806,25 +1823,25 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="I15" s="3"/>
     </row>
@@ -1833,25 +1850,25 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="I16" s="3"/>
     </row>
@@ -1860,25 +1877,25 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>31</v>
+        <v>232</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="I17" s="3"/>
     </row>
@@ -1887,25 +1904,25 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="I18" s="3"/>
     </row>
@@ -1914,25 +1931,25 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="I19" s="3"/>
     </row>
@@ -1941,25 +1958,25 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="I20" s="3"/>
     </row>
@@ -1968,25 +1985,25 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="I21" s="3"/>
     </row>
@@ -1995,25 +2012,25 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="I22" s="3"/>
     </row>
@@ -2022,25 +2039,25 @@
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>38</v>
+        <v>233</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="I23" s="3"/>
     </row>
@@ -2049,25 +2066,25 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>39</v>
+        <v>24</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="I24" s="3"/>
     </row>
@@ -2076,25 +2093,25 @@
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>40</v>
+        <v>14</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>238</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="I25" s="3"/>
     </row>
@@ -2103,25 +2120,25 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="I26" s="3"/>
     </row>
@@ -2130,25 +2147,25 @@
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="I27" s="3"/>
     </row>
@@ -2157,25 +2174,25 @@
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>43</v>
+        <v>25</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>234</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="I28" s="3"/>
     </row>
@@ -2184,25 +2201,25 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="I29" s="3"/>
     </row>
@@ -2211,25 +2228,25 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="I30" s="3"/>
     </row>
@@ -2238,23 +2255,25 @@
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D31" s="3"/>
+      <c r="D31" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="E31" s="3" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="I31" s="3"/>
     </row>
@@ -2263,25 +2282,25 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>46</v>
+        <v>237</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="I32" s="3"/>
     </row>
@@ -2290,25 +2309,25 @@
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="I33" s="3"/>
     </row>
@@ -2317,25 +2336,25 @@
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="I34" s="3"/>
     </row>
@@ -2344,25 +2363,25 @@
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="I35" s="3"/>
     </row>
@@ -2371,25 +2390,25 @@
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="I36" s="3"/>
     </row>
@@ -2398,25 +2417,25 @@
         <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="I37" s="3"/>
     </row>
@@ -2425,25 +2444,25 @@
         <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>53</v>
+        <v>235</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="I38" s="3"/>
     </row>
@@ -2452,25 +2471,25 @@
         <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="I39" s="3"/>
     </row>
@@ -2479,25 +2498,25 @@
         <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="I40" s="3"/>
     </row>
@@ -2506,25 +2525,25 @@
         <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>56</v>
+        <v>236</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="I41" s="3"/>
     </row>
@@ -2533,28 +2552,28 @@
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
@@ -2562,28 +2581,28 @@
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
@@ -2591,28 +2610,28 @@
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
@@ -2620,25 +2639,25 @@
         <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="I45" s="3"/>
     </row>
@@ -2647,25 +2666,25 @@
         <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="I46" s="3"/>
     </row>
@@ -2674,25 +2693,25 @@
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>63</v>
+        <v>239</v>
       </c>
       <c r="E47" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F47" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="F47" s="3" t="s">
-        <v>135</v>
-      </c>
       <c r="G47" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="I47" s="3"/>
     </row>
@@ -2701,25 +2720,25 @@
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="I48" s="3"/>
     </row>
@@ -2728,25 +2747,25 @@
         <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D49" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C49" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>65</v>
-      </c>
       <c r="E49" s="3" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="I49" s="3"/>
     </row>
@@ -2755,28 +2774,28 @@
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
@@ -2784,28 +2803,28 @@
         <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
@@ -2813,28 +2832,28 @@
         <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
@@ -2842,28 +2861,28 @@
         <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
@@ -2871,28 +2890,28 @@
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
@@ -2900,28 +2919,28 @@
         <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
@@ -2929,28 +2948,28 @@
         <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
@@ -2958,28 +2977,28 @@
         <v>56</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
@@ -2987,28 +3006,28 @@
         <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="I58" s="3" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
@@ -3016,28 +3035,28 @@
         <v>58</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
@@ -3045,28 +3064,28 @@
         <v>59</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
@@ -3074,28 +3093,28 @@
         <v>61</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
@@ -3103,28 +3122,28 @@
         <v>60</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="I62" s="3" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
@@ -3132,28 +3151,28 @@
         <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
@@ -3161,32 +3180,32 @@
         <v>63</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="I64" s="3" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I64"/>
+  <autoFilter ref="A1:I64" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3194,10 +3213,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -3213,10 +3232,10 @@
         <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -3227,227 +3246,227 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="66" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B3" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="B4" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B5" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C5" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="33" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B6" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="B7" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B8" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="33" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="B9" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="33" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="B10" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="B11" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="B12" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="B13" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="33" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="B14" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="33" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="B15" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="33" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="B16" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="66" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="B17" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="66" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="B18" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B19" t="s">
+        <v>203</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="33" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="B20" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="33" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="B21" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="B22" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -3461,7 +3480,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3479,31 +3498,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="84.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>